<commit_message>
UML Arrangement 2022/02/11 Sian-Xia
</commit_message>
<xml_diff>
--- a/UML/PETHOTEL_UML_.xlsx
+++ b/UML/PETHOTEL_UML_.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24930" windowHeight="10610" firstSheet="4"/>
+    <workbookView windowWidth="21030" windowHeight="10610" firstSheet="4" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UML" sheetId="3" r:id="rId1"/>
@@ -62,9 +62,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -98,9 +98,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,16 +111,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,12 +136,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,7 +172,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -172,10 +188,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -188,14 +204,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
@@ -204,25 +212,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -235,7 +228,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,6 +236,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,7 +263,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,7 +299,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,13 +359,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,61 +389,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,13 +407,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,25 +425,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,25 +437,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,11 +537,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,6 +563,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,6 +602,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -596,32 +622,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,148 +639,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3649,326 +3649,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>613410</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>134620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>487045</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>141605</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="菱形 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6557010" y="2268220"/>
-          <a:ext cx="1854835" cy="1073785"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="zh-CN">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-            </a:defRPr>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="zh-CN" sz="1100"/>
-            <a:t>チェックイン</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>628015</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>130175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>501650</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="菱形 7"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6571615" y="3508375"/>
-          <a:ext cx="1854835" cy="1073785"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="zh-CN">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-            </a:defRPr>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>2</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="zh-CN" sz="1100"/>
-            <a:t>チェックアウト</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
       <xdr:colOff>605790</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
@@ -4124,326 +3804,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>647065</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="菱形 9"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6590665" y="4778375"/>
-          <a:ext cx="1854835" cy="1073785"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="zh-CN">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-            </a:defRPr>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>3</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="zh-CN" sz="1100"/>
-            <a:t>空き部屋検査</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>661035</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>534670</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>93345</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="菱形 10"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6604000" y="6130925"/>
-          <a:ext cx="1855470" cy="1074420"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="zh-CN">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-            </a:defRPr>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>4</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="zh-CN" sz="1100"/>
-            <a:t>予約</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>194310</xdr:colOff>
       <xdr:row>4</xdr:row>
@@ -4467,940 +3827,6 @@
         <a:xfrm>
           <a:off x="7458710" y="746125"/>
           <a:ext cx="16510" cy="153035"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>17145</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>134620</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="直接箭头连接符 13"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="2"/>
-          <a:endCxn id="7" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7477760" y="1972945"/>
-          <a:ext cx="7620" cy="295275"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>141605</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>235585</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>130175</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="直接箭头连接符 14"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="7" idx="2"/>
-          <a:endCxn id="8" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7485380" y="3342005"/>
-          <a:ext cx="14605" cy="166370"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>233045</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>55880</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="直接箭头连接符 15"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="8" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7497445" y="4581525"/>
-          <a:ext cx="27305" cy="274955"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>254635</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>267970</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="直接箭头连接符 16"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="2"/>
-          <a:endCxn id="11" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7519035" y="5852160"/>
-          <a:ext cx="13335" cy="278765"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>76835</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>62230</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>89535</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="直接箭头连接符 17"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="11" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5360035" y="6640830"/>
-          <a:ext cx="1243965" cy="27305"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>97790</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161290</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>189230</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>76835</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="19" name="直接箭头连接符 18"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5380990" y="694690"/>
-          <a:ext cx="91440" cy="5960745"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>203835</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>4445</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>118745</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="直接箭头连接符 19"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5487035" y="715645"/>
-          <a:ext cx="1974215" cy="114300"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>154305</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>147320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>598805</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4445</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="直接箭头连接符 21"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5437505" y="2814320"/>
-          <a:ext cx="1104900" cy="34925"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>111760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>628015</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="直接箭头连接符 22"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="8" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5416550" y="4023360"/>
-          <a:ext cx="1155065" cy="21590"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>97790</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>154305</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>647065</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="24" name="直接箭头连接符 23"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5380990" y="5310505"/>
-          <a:ext cx="1209675" cy="4445"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>636270</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>509905</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>153670</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="菱形 25"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6579870" y="7613650"/>
-          <a:ext cx="1854835" cy="1074420"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="zh-CN">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-            </a:defRPr>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>5</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="zh-CN" sz="1100"/>
-            <a:t>予約キャンセル</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>93345</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>267970</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="直接箭头连接符 26"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="11" idx="2"/>
-          <a:endCxn id="26" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7508240" y="7205345"/>
-          <a:ext cx="24130" cy="408305"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>625475</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="直接箭头连接符 27"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5337175" y="8201025"/>
-          <a:ext cx="1231900" cy="15875"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>93980</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>141605</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="直接箭头连接符 28"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5377180" y="6632575"/>
-          <a:ext cx="7620" cy="1510030"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>479425</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>538480</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>13970</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="直接箭头连接符 29"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="3"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8404225" y="1409700"/>
-          <a:ext cx="1379855" cy="26670"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>474980</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="直接箭头连接符 30"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9601200" y="1452880"/>
-          <a:ext cx="119380" cy="8249920"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>347980</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp>
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="直接箭头连接符 31"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7651750" y="9655175"/>
-          <a:ext cx="1941830" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5540,6 +3966,1297 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>205105</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>78105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>570230</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>128905</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9450705" y="2389505"/>
+          <a:ext cx="1685925" cy="939800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="2400">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="zh-CN" sz="2400">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>チェックイン</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>191770</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>58420</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>556895</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>109220</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9437370" y="3792220"/>
+          <a:ext cx="1685925" cy="939800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="zh-CN" sz="2400">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>チェックアウト</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9429750" y="5124450"/>
+          <a:ext cx="1685925" cy="939800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="2400">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="zh-CN" sz="2400">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>空き部屋検査</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>525145</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>93980</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="矩形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9405620" y="6443980"/>
+          <a:ext cx="1685925" cy="939800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="2600">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>4</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="zh-CN" sz="2600">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>予約</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>151765</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>516890</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="矩形 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9397365" y="7727950"/>
+          <a:ext cx="1685925" cy="939800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="zh-CN">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="2400">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="zh-CN" sz="2400">
+              <a:sym typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t>予約キャンセル</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>34290</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>17145</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38735</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直接箭头连接符 20"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="2"/>
+          <a:endCxn id="33" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7298690" y="1972945"/>
+          <a:ext cx="179070" cy="7311390"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>479425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>13970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>205105</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>16510</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直接连接符 24"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8404225" y="1436370"/>
+          <a:ext cx="1046480" cy="1424940"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>474980</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>191770</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="直接箭头连接符 34"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8399780" y="1444625"/>
+          <a:ext cx="1037590" cy="2816225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>479425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>13970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>205105</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="直接箭头连接符 35"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8404225" y="1436370"/>
+          <a:ext cx="1046480" cy="4259580"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>490855</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直接箭头连接符 36"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8415655" y="1476375"/>
+          <a:ext cx="989965" cy="5436235"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>498475</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>151765</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="直接箭头连接符 37"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="12" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8423275" y="1476375"/>
+          <a:ext cx="974090" cy="6723380"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>506730</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46355</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>570230</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>16510</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="曲线连接符 38"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8431530" y="1468755"/>
+          <a:ext cx="2705100" cy="1392555"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -8824"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>467360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="曲线连接符 39"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8392160" y="1452880"/>
+          <a:ext cx="2660015" cy="2776220"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -52045"/>
+            <a:gd name="adj2" fmla="val 123970"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>479425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>13970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="曲线连接符 40"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="3"/>
+          <a:endCxn id="9" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8404225" y="1436370"/>
+          <a:ext cx="2711450" cy="4157980"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -129976"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>525145</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="曲线连接符 41"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8375650" y="1524000"/>
+          <a:ext cx="2715895" cy="5388610"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -99015"/>
+            <a:gd name="adj2" fmla="val 104882"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>474980</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>78105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>516890</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="曲线连接符 42"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8399780" y="1500505"/>
+          <a:ext cx="2683510" cy="6699250"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -158918"/>
+            <a:gd name="adj2" fmla="val 107915"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -10098,7 +9815,7 @@
   <sheetPr/>
   <dimension ref="D2:BF82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BB8" sqref="BB8"/>
     </sheetView>
   </sheetViews>
@@ -13949,8 +13666,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -14027,7 +13744,7 @@
   <sheetPr/>
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>

</xml_diff>